<commit_message>
Experiment updates, Hyperparameter Tuning fix
</commit_message>
<xml_diff>
--- a/DeepESN/DO_Permutation_Results.xlsx
+++ b/DeepESN/DO_Permutation_Results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="model_summaries" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="model_summaries" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -558,7 +558,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'epochs': 50}</t>
+          <t>{'batch_size': 16, 'epochs': 50, 'layers_struct': [{'units': 150, 'dropout': 0.4}, {'units': 100, 'dropout': 0.3}, {'units': 50, 'dropout': 0.2}]}</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -573,36 +573,42 @@
       <c r="H2" t="n">
         <v>0.95</v>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>0.08771346807479929</v>
+      </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="b">
         <v>1</v>
       </c>
       <c r="N2" t="n">
-        <v>1.45488614747484</v>
+        <v>1.390577358120786</v>
       </c>
       <c r="O2" t="n">
-        <v>0.1062538737182223</v>
+        <v>0.1016039392577006</v>
       </c>
       <c r="P2" t="n">
-        <v>1.046974690741037</v>
+        <v>1.001877508455949</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.4568547041333999</v>
+        <v>0.5038096515647162</v>
       </c>
       <c r="R2" t="n">
-        <v>0.8155294473187785</v>
+        <v>0.8316726753171663</v>
       </c>
       <c r="S2" t="n">
-        <v>0.06647867757161968</v>
+        <v>0.06656464121876902</v>
       </c>
       <c r="T2" t="n">
-        <v>0.6569970851937931</v>
+        <v>0.6604753503600755</v>
       </c>
       <c r="U2" t="n">
-        <v>0.8453699573273429</v>
+        <v>0.8391876319974456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>